<commit_message>
typo in table 6.0 fixed
</commit_message>
<xml_diff>
--- a/model/Metanproduktion_Arrhenius_v8_30012024_efter_rettelse_fra_fagfællebedømmelse.xlsx
+++ b/model/Metanproduktion_Arrhenius_v8_30012024_efter_rettelse_fra_fagfællebedømmelse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au277187_uni_au_dk/Documents/Documents/GitHub/AU-BCE-EE/Dalby-2024-KVIK/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{A03A6902-9A89-4468-8B98-E20900CA048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E84F47-69FF-41BD-952C-FEC682C34160}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{A03A6902-9A89-4468-8B98-E20900CA048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FB56BB4-F6C3-46F3-989A-C1D6B844A1A1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel_svin" sheetId="1" r:id="rId1"/>
@@ -2603,19 +2603,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="6" topLeftCell="AJ21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="AJ28" sqref="AJ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="14" width="27.85546875" style="2" customWidth="1"/>
     <col min="15" max="15" width="29.42578125" style="2" customWidth="1"/>
     <col min="16" max="16" width="28" style="2" bestFit="1" customWidth="1"/>
@@ -56009,7 +56009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -58849,14 +58849,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="51017e06-3185-4484-8ddc-2b23098c8f10" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd6032e-4b27-47f4-bb02-403eeb79ffb0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59065,21 +59063,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="51017e06-3185-4484-8ddc-2b23098c8f10" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd6032e-4b27-47f4-bb02-403eeb79ffb0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE2544F1-D550-4ABD-8DC3-837C3181A044}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B591A28-77E8-4B69-8E3E-D2C48B98FB73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51017e06-3185-4484-8ddc-2b23098c8f10"/>
-    <ds:schemaRef ds:uri="0cd6032e-4b27-47f4-bb02-403eeb79ffb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -59104,9 +59101,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B591A28-77E8-4B69-8E3E-D2C48B98FB73}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE2544F1-D550-4ABD-8DC3-837C3181A044}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51017e06-3185-4484-8ddc-2b23098c8f10"/>
+    <ds:schemaRef ds:uri="0cd6032e-4b27-47f4-bb02-403eeb79ffb0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>